<commit_message>
Got averaging for headings working
</commit_message>
<xml_diff>
--- a/logs/PID tuning.xlsx
+++ b/logs/PID tuning.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="1200" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="8840" yWindow="1160" windowWidth="34100" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="PID tuning.csv" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -150,7 +150,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -161,7 +161,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>'PID tuning.csv'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -194,7 +194,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$67</c:f>
+              <c:f>'PID tuning.csv'!$J$2:$J$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -403,7 +403,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'PID tuning.csv'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -436,7 +436,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$67</c:f>
+              <c:f>'PID tuning.csv'!$F$2:$F$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -659,7 +659,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>'PID tuning.csv'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -692,7 +692,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$67</c:f>
+              <c:f>'PID tuning.csv'!$M$2:$M$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -914,20 +914,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1098,6 +1084,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>

</xml_diff>